<commit_message>
Adding some basic sketches of site template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\git\basic-css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.garisch\Desktop\git\basic-css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DD5E90B9-68A2-40A9-B7BA-E29C5F676A7D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F396BA8E-148B-4412-BCC3-8CFA80E71581}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13392" xr2:uid="{C4DA3095-A914-432F-9950-E755B3AEDCDD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13392" activeTab="3" xr2:uid="{C4DA3095-A914-432F-9950-E755B3AEDCDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
     <sheet name="Desktop" sheetId="1" r:id="rId2"/>
     <sheet name="Mobile" sheetId="2" r:id="rId3"/>
+    <sheet name="Desktop2" sheetId="4" r:id="rId4"/>
+    <sheet name="Mobile2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>5 by 5</t>
   </si>
@@ -198,6 +200,57 @@
   </si>
   <si>
     <t>Java</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Exercises</t>
+  </si>
+  <si>
+    <t>Nav Burger</t>
+  </si>
+  <si>
+    <t>A bootstrap 4 carousel with comments about the course</t>
+  </si>
+  <si>
+    <t>This will only be for the landing page at this stage</t>
+  </si>
+  <si>
+    <t>Nav 'Capstone'</t>
+  </si>
+  <si>
+    <t>Exercises Navigation</t>
+  </si>
+  <si>
+    <t>Vertical for large view</t>
+  </si>
+  <si>
+    <t>Horizontal for medium or smaller view</t>
+  </si>
+  <si>
+    <t>Jumbotron exercise description</t>
+  </si>
+  <si>
+    <t>Exercise solutions</t>
+  </si>
+  <si>
+    <t>We'll use Bootstrap 4 as the css framework, not BS3.</t>
+  </si>
+  <si>
+    <t>This site will demonstrate practicing JS programming</t>
+  </si>
+  <si>
+    <t>with the use of exercises from project Euler.</t>
+  </si>
+  <si>
+    <t>highlight.js will be used for code syntax highlighting.</t>
+  </si>
+  <si>
+    <t>Collapses &lt; md view</t>
   </si>
 </sst>
 </file>
@@ -280,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -303,11 +356,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -324,6 +457,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -642,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0486A15-2E4C-46DC-B7FA-91299B61240E}">
   <dimension ref="B2:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3159,4 +3308,621 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A01D9C0-2703-4106-815B-CD36CE52E4BC}">
+  <dimension ref="B1:S29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="16"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="16"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="19"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="S3" s="19"/>
+    </row>
+    <row r="4" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="S4" s="22"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="16"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="16"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="19"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="19"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="19"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="19"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="19"/>
+    </row>
+    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="22"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" s="14"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+      <c r="L12" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15">
+        <v>1</v>
+      </c>
+      <c r="O12" s="15">
+        <v>2</v>
+      </c>
+      <c r="P12" s="15">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="15">
+        <v>4</v>
+      </c>
+      <c r="R12" s="15">
+        <v>5</v>
+      </c>
+      <c r="S12" s="16"/>
+    </row>
+    <row r="13" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="19"/>
+      <c r="L13" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="22"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>7</v>
+      </c>
+      <c r="R13" s="21">
+        <v>8</v>
+      </c>
+      <c r="S13" s="22"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B14" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="19"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="16"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B15" s="17">
+        <v>1</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="19"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="19"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B16" s="17">
+        <v>2</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="19"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="19"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B17" s="17">
+        <v>3</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="19"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="19"/>
+    </row>
+    <row r="18" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="17">
+        <v>4</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="22"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="22"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B19" s="17">
+        <v>5</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="19"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="19"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B20" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="19"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="19"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B21" s="17"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="19"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="19"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B22" s="17"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="19"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="19"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B23" s="17"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="19"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="19"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B24" s="17"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="19"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="19"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B25" s="17"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="19"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="19"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B26" s="17"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="19"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="19"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B27" s="17"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="19"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="19"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B28" s="17"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="19"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="19"/>
+    </row>
+    <row r="29" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="20"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="22"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B1D212-339A-49CF-B9DB-C3D0E158D062}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>